<commit_message>
More products service unit tests
</commit_message>
<xml_diff>
--- a/src/Web/WHMS.Web/wwwroot/ExcelUploads/OrdersImportTemplate.xlsx
+++ b/src/Web/WHMS.Web/wwwroot/ExcelUploads/OrdersImportTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jivko\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WHMS\src\Web\WHMS.Web\wwwroot\ExcelUploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E747E834-66C1-476A-9ED4-0FCC3F81B63C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE00211-127A-40F0-92FF-FAE2A41E9B95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="1170" windowWidth="28680" windowHeight="11550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="2340" windowWidth="28680" windowHeight="11550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>SourceOrderId</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Zip</t>
+  </si>
+  <si>
+    <t>Channel</t>
   </si>
 </sst>
 </file>
@@ -378,60 +381,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>